<commit_message>
Flight Finder & Select Flight Test Done
</commit_message>
<xml_diff>
--- a/src/main/java/data.xlsx
+++ b/src/main/java/data.xlsx
@@ -4,20 +4,33 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8030" windowHeight="2840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21990" windowHeight="12990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="excellogin" sheetId="1" r:id="rId1"/>
+    <sheet name="FlightFinder" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H8"/>
+  <oleSize ref="A1:W15"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>tutorial</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Unified Airlines</t>
   </si>
 </sst>
 </file>
@@ -361,16 +374,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>